<commit_message>
['22] bugfix drgl 93xx
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3052314B-9DC3-40EE-A93B-F821F7F2531C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE44BB50-C1ED-45AD-BEFD-5DFAA4115D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9203" yWindow="4500" windowWidth="14401" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
['22] overzicht goederentreinen RM391
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE44BB50-C1ED-45AD-BEFD-5DFAA4115D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0C49DC-48BA-4582-AFBA-9BD2137DCD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9203" yWindow="4500" windowWidth="14401" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="14400" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ZWNL Treinseries" sheetId="1" r:id="rId1"/>
+    <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
+    <sheet name="ZWNL Treinseries" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ZWNL Treinseries'!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ZWNL Treinseries'!$A$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,6 +29,64 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{68424BFA-189C-4F56-AB72-14697606771B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Pad nodig ri amsterdam!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{4888225A-AFCF-4B44-A5DA-74E8E8AAC3E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TODO: FS ook toevoegen Amf-Apd!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tom</author>
@@ -86,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="119">
   <si>
     <t>Treinserie</t>
   </si>
@@ -215,6 +274,235 @@
   </si>
   <si>
     <t>Freight Coal</t>
+  </si>
+  <si>
+    <t>Bron</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>ZWNL</t>
+  </si>
+  <si>
+    <t>HVNL</t>
+  </si>
+  <si>
+    <t>ZvNL</t>
+  </si>
+  <si>
+    <t>Lovosice Shuttle</t>
+  </si>
+  <si>
+    <t>Vervoerder</t>
+  </si>
+  <si>
+    <t>CD Cargo</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>BR/Bh-Erp</t>
+  </si>
+  <si>
+    <t>FG, FCl</t>
+  </si>
+  <si>
+    <t>FCr</t>
+  </si>
+  <si>
+    <t>FCr, FW</t>
+  </si>
+  <si>
+    <t>RM391p17, TP</t>
+  </si>
+  <si>
+    <t>Moers-kolentrein</t>
+  </si>
+  <si>
+    <t>NIAG</t>
+  </si>
+  <si>
+    <t>Mvt/Awhv-BR?</t>
+  </si>
+  <si>
+    <t>FCl*</t>
+  </si>
+  <si>
+    <t>Pon autotrein</t>
+  </si>
+  <si>
+    <t>HSL</t>
+  </si>
+  <si>
+    <t>Amf-Bh</t>
+  </si>
+  <si>
+    <t>RM391p18, TP</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>DBC</t>
+  </si>
+  <si>
+    <t>Kolen OBA-Frankfurt</t>
+  </si>
+  <si>
+    <t>RM391p19</t>
+  </si>
+  <si>
+    <t>Hrp-?</t>
+  </si>
+  <si>
+    <t>LTE</t>
+  </si>
+  <si>
+    <t>Coevorden shuttle</t>
+  </si>
+  <si>
+    <t>IRP?</t>
+  </si>
+  <si>
+    <t>Co-Zl-Wp-Mvt</t>
+  </si>
+  <si>
+    <t>RM391p19, TP</t>
+  </si>
+  <si>
+    <t>FW</t>
+  </si>
+  <si>
+    <t>P&amp;O Novara shuttle</t>
+  </si>
+  <si>
+    <t>BLSC &lt;SBBC</t>
+  </si>
+  <si>
+    <t>Erp-BR</t>
+  </si>
+  <si>
+    <t>Rheinhausen shuttle</t>
+  </si>
+  <si>
+    <t>LNS</t>
+  </si>
+  <si>
+    <t>Mvt-BR</t>
+  </si>
+  <si>
+    <t>RM391p20, TP</t>
+  </si>
+  <si>
+    <t>Strasbourg/Kehl shuttle</t>
+  </si>
+  <si>
+    <t>GTS shuttle</t>
+  </si>
+  <si>
+    <t>SBBC</t>
+  </si>
+  <si>
+    <t>Bot-Vl?</t>
+  </si>
+  <si>
+    <t>RM391p21, TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>Rotterdam Xpress?</t>
+  </si>
+  <si>
+    <t>Mvt-Atw</t>
+  </si>
+  <si>
+    <t>RM391p21, TP?</t>
+  </si>
+  <si>
+    <t>FL, FCl*</t>
+  </si>
+  <si>
+    <t>Styreen Terneuzen?</t>
+  </si>
+  <si>
+    <t>B-Rsd-Kfh</t>
+  </si>
+  <si>
+    <t>RFO</t>
+  </si>
+  <si>
+    <t>Kfh-Bh</t>
+  </si>
+  <si>
+    <t>RM391p21</t>
+  </si>
+  <si>
+    <t>FCl</t>
+  </si>
+  <si>
+    <t>Dillingen-ertstrein</t>
+  </si>
+  <si>
+    <t>Mvt/Sloe-Vl</t>
+  </si>
+  <si>
+    <t>FP, FN</t>
+  </si>
+  <si>
+    <t>Tb-Ehv-Vl</t>
+  </si>
+  <si>
+    <t>Westports-Express</t>
+  </si>
+  <si>
+    <t>RM391p22, TP</t>
+  </si>
+  <si>
+    <t>Cargobeamer</t>
+  </si>
+  <si>
+    <t>Wzh: Rsd-Vl</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>Curtici (spottransport)</t>
+  </si>
+  <si>
+    <t>RTBC</t>
+  </si>
+  <si>
+    <t>Sloe-Vl</t>
+  </si>
+  <si>
+    <t>RM391p22</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>Craiova Ford autotrein</t>
+  </si>
+  <si>
+    <t>Sitfa Ford autotrein</t>
+  </si>
+  <si>
+    <t>Mat'64 904</t>
+  </si>
+  <si>
+    <t>CREW</t>
+  </si>
+  <si>
+    <t>RM391p23</t>
+  </si>
+  <si>
+    <t>Amf-Hdr;
+Gvc-Ut-Ah-Amf</t>
   </si>
 </sst>
 </file>
@@ -259,12 +547,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -279,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -288,6 +582,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,10 +874,427 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345995E5-71C5-4554-A66C-476FDA92E42E}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18" style="6" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Overzicht treinseries HSL 2022
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E283BF3-5875-4250-B9F8-3E71C8E25B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79E62E0-17B0-4049-99A0-93990371AFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7095" yWindow="2370" windowWidth="14400" windowHeight="7485" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
     <sheet name="ZWNL Treinseries" sheetId="1" r:id="rId2"/>
     <sheet name="ZWNL Goederenverbindingen" sheetId="4" r:id="rId3"/>
     <sheet name="ZvNL Treinseries" sheetId="3" r:id="rId4"/>
+    <sheet name="HSL Treinseries" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZvNL Treinseries'!$A$1:$F$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL Goederenverbindingen'!$A$20:$E$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ZWNL Treinseries'!$A$1:$F$30</definedName>
@@ -322,8 +324,42 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D572B1D8-0BA2-43D9-A778-E3F279018DD7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+losse uitzonderingen weggelaten!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="192">
   <si>
     <t>Treinserie</t>
   </si>
@@ -864,6 +900,42 @@
   </si>
   <si>
     <t>Sloe - Esn</t>
+  </si>
+  <si>
+    <t>IC Berlijn</t>
+  </si>
+  <si>
+    <t>Min bak</t>
+  </si>
+  <si>
+    <t>VIRM</t>
+  </si>
+  <si>
+    <t>ICRmh</t>
+  </si>
+  <si>
+    <t>DDZ, ICM</t>
+  </si>
+  <si>
+    <t>0.6, 0.4</t>
+  </si>
+  <si>
+    <t>Passenger Scrap, Intercity</t>
+  </si>
+  <si>
+    <t>VIRM?</t>
+  </si>
+  <si>
+    <t>SNG?</t>
+  </si>
+  <si>
+    <t>SLT?</t>
+  </si>
+  <si>
+    <t>Blindzug</t>
+  </si>
+  <si>
+    <t>Custom 8</t>
   </si>
 </sst>
 </file>
@@ -2207,7 +2279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA394F4-D495-45BA-A765-8FE37C144B84}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2431,7 +2503,7 @@
         <v>9300</v>
       </c>
       <c r="D21" s="15">
-        <f>C21/(B21*24*250)</f>
+        <f t="shared" ref="D21:D30" si="0">C21/(B21*24*250)</f>
         <v>0.31</v>
       </c>
       <c r="E21" t="s">
@@ -2450,7 +2522,7 @@
         <v>6250</v>
       </c>
       <c r="D22" s="15">
-        <f>C22/(B22*24*250)</f>
+        <f t="shared" si="0"/>
         <v>0.34722222222222221</v>
       </c>
       <c r="E22" t="s">
@@ -2469,7 +2541,7 @@
         <v>2850</v>
       </c>
       <c r="D23" s="15">
-        <f>C23/(B23*24*250)</f>
+        <f t="shared" si="0"/>
         <v>0.23749999999999999</v>
       </c>
       <c r="E23" t="s">
@@ -2488,7 +2560,7 @@
         <v>2050</v>
       </c>
       <c r="D24" s="15">
-        <f>C24/(B24*24*250)</f>
+        <f t="shared" si="0"/>
         <v>0.11388888888888889</v>
       </c>
       <c r="E24" t="s">
@@ -2506,7 +2578,7 @@
         <v>1550</v>
       </c>
       <c r="D25" s="15">
-        <f>C25/(B25*24*250)</f>
+        <f t="shared" si="0"/>
         <v>8.611111111111111E-2</v>
       </c>
       <c r="E25" t="s">
@@ -2524,7 +2596,7 @@
         <v>1100</v>
       </c>
       <c r="D26" s="15">
-        <f>C26/(B26*24*250)</f>
+        <f t="shared" si="0"/>
         <v>2.6190476190476191E-2</v>
       </c>
       <c r="E26" t="s">
@@ -2543,7 +2615,7 @@
         <v>1100</v>
       </c>
       <c r="D27" s="15">
-        <f>C27/(B27*24*250)</f>
+        <f t="shared" si="0"/>
         <v>0.18333333333333332</v>
       </c>
       <c r="E27" t="s">
@@ -2561,7 +2633,7 @@
         <v>550</v>
       </c>
       <c r="D28" s="15">
-        <f>C28/(B28*24*250)</f>
+        <f t="shared" si="0"/>
         <v>9.166666666666666E-2</v>
       </c>
       <c r="E28" t="s">
@@ -2580,7 +2652,7 @@
         <v>350</v>
       </c>
       <c r="D29" s="15">
-        <f>C29/(B29*24*250)</f>
+        <f t="shared" si="0"/>
         <v>1.4583333333333334E-2</v>
       </c>
       <c r="E29" t="s">
@@ -2598,7 +2670,7 @@
         <v>200</v>
       </c>
       <c r="D30" s="15">
-        <f>C30/(B30*24*250)</f>
+        <f t="shared" si="0"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="E30" t="s">
@@ -2622,7 +2694,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3145,4 +3217,805 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
+  <dimension ref="A1:G46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="10.53125" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="19.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>500</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>600</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>700</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>800</v>
+      </c>
+      <c r="B7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>900</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>1100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>1500</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>1600</v>
+      </c>
+      <c r="B12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>1800</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>2100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>2200</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>2400</v>
+      </c>
+      <c r="B16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>2600</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>2800</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2900</v>
+      </c>
+      <c r="B19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>3000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>3100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>3200</v>
+      </c>
+      <c r="B22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>3300</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>3500</v>
+      </c>
+      <c r="B24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>3700</v>
+      </c>
+      <c r="B25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>3900</v>
+      </c>
+      <c r="B26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>4000</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>4300</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>4500</v>
+      </c>
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>4600</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>4800</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>5000</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>5100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>5200</v>
+      </c>
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>5400</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>5700</v>
+      </c>
+      <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>141</v>
+      </c>
+      <c r="G36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>5800</v>
+      </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>7400</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>7700</v>
+      </c>
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>9100</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>9200</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>9300</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>11600</v>
+      </c>
+      <c r="B43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>186</v>
+      </c>
+      <c r="G43" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>14600</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>15800</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>190</v>
+      </c>
+      <c r="E46" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G8" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G45">
+      <sortCondition ref="A1:A8"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[HSL] drgl research and consists
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79E62E0-17B0-4049-99A0-93990371AFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E463307-6F9D-4AE6-95A1-456C042162D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5790" yWindow="2348" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ZWNL Goederenverbindingen" sheetId="4" r:id="rId3"/>
     <sheet name="ZvNL Treinseries" sheetId="3" r:id="rId4"/>
     <sheet name="HSL Treinseries" sheetId="5" r:id="rId5"/>
+    <sheet name="HSL Scenarios" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
@@ -359,7 +360,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="200">
   <si>
     <t>Treinserie</t>
   </si>
@@ -932,10 +933,35 @@
     <t>SLT?</t>
   </si>
   <si>
-    <t>Blindzug</t>
-  </si>
-  <si>
-    <t>Custom 8</t>
+    <t>Naam</t>
+  </si>
+  <si>
+    <t>Player spawn</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Statisch</t>
+  </si>
+  <si>
+    <t>Treinen vóór speler</t>
+  </si>
+  <si>
+    <t>Altijd-rood</t>
+  </si>
+  <si>
+    <t>Timers</t>
+  </si>
+  <si>
+    <t>- Hfdm MDWVZ</t>
+  </si>
+  <si>
+    <t>Hfd:
+- asdas</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1063,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1066,6 +1092,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -3221,11 +3250,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3264,160 +3293,184 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>100</v>
+        <v>1600</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
+        <v>184</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>186</v>
+      </c>
+      <c r="F2">
+        <f>2*85</f>
+        <v>170</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>140</v>
+        <v>11600</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>184</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>186</v>
+      </c>
+      <c r="F3">
+        <f>2*85</f>
+        <v>170</v>
+      </c>
+      <c r="G3" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>500</v>
+        <v>9100</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>600</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
+        <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>700</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>800</v>
+        <v>2600</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <f>2*110</f>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="F8">
+        <f>110+85</f>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="F9">
+        <f>110+85</f>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>1100</v>
+        <v>1500</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>6</v>
       </c>
       <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
         <v>7</v>
       </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="F10">
+        <f>110+85</f>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -3425,36 +3478,41 @@
       <c r="E11" t="s">
         <v>27</v>
       </c>
+      <c r="F11">
+        <f>110+85</f>
+        <v>195</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="B12" t="s">
-        <v>184</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>186</v>
-      </c>
-      <c r="G12" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="F12">
+        <f>110+85</f>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>1800</v>
+        <v>2800</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -3462,246 +3520,290 @@
       <c r="E13" t="s">
         <v>27</v>
       </c>
+      <c r="F13">
+        <f>110+85</f>
+        <v>195</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>2100</v>
+        <v>1100</v>
       </c>
       <c r="B14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>2200</v>
+        <v>9200</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>2400</v>
+        <v>900</v>
       </c>
       <c r="B16" t="s">
-        <v>187</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>2600</v>
+        <v>1000</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>2800</v>
+        <v>7400</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+      <c r="F18">
+        <f>2*105</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>2900</v>
+        <v>4000</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+      <c r="F19">
+        <f>105+75</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>3000</v>
+        <v>4800</v>
       </c>
       <c r="B20" t="s">
-        <v>182</v>
+        <v>15</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+      <c r="F20">
+        <f>105+75</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21">
-        <v>3100</v>
+        <v>5400</v>
       </c>
       <c r="B21" t="s">
-        <v>182</v>
+        <v>15</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+      <c r="F21">
+        <f>105+75</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
-        <v>3200</v>
+        <v>5700</v>
       </c>
       <c r="B22" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="F22">
+        <f>2*80</f>
+        <v>160</v>
+      </c>
+      <c r="G22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23">
+        <v>7700</v>
+      </c>
+      <c r="B23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23">
+        <f>2*105</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>14600</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24">
+        <f>2*80+65</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>4600</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25">
+        <f>2*80+65</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26">
         <v>3300</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>16</v>
       </c>
-      <c r="C23">
+      <c r="C26">
         <v>3</v>
       </c>
-      <c r="D23">
+      <c r="D26">
         <v>8</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>3500</v>
-      </c>
-      <c r="B24" t="s">
-        <v>182</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>3700</v>
-      </c>
-      <c r="B25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>3900</v>
-      </c>
-      <c r="B26" t="s">
-        <v>182</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F26">
+        <f>2*80</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>4000</v>
+        <v>5100</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <f>2*80</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>4300</v>
       </c>
@@ -3717,242 +3819,301 @@
       <c r="E28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F28">
+        <f>65+80</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>4500</v>
+        <v>5000</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="F29">
+        <f>65+80</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>4600</v>
+        <v>5800</v>
       </c>
       <c r="B30" t="s">
         <v>16</v>
       </c>
       <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
         <v>7</v>
-      </c>
-      <c r="D30">
-        <v>11</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F30">
+        <f>65+80</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31">
-        <v>4800</v>
+        <v>15800</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C31">
         <v>6</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="F31">
+        <f>65+80</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>5000</v>
+        <v>5200</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>188</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D32">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F32">
+        <f>2*80</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>5100</v>
+        <v>9300</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33">
-        <v>7</v>
-      </c>
-      <c r="D33">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
-        <v>5200</v>
+        <v>2100</v>
       </c>
       <c r="B34" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D34">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F34">
+        <f>115+170</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <v>5400</v>
+        <v>2200</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>182</v>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D35">
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F35">
+        <f>115+170</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>5700</v>
+        <v>3000</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
       <c r="D36">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>141</v>
-      </c>
-      <c r="G36" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F36">
+        <f>115+170</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>5800</v>
+        <v>800</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>182</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F37">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
-        <v>7400</v>
+        <v>2900</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>182</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D38">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F38">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>7700</v>
+        <v>3100</v>
       </c>
       <c r="B39" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D39">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F39">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>9100</v>
+        <v>3200</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>182</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F40">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <v>9200</v>
+        <v>3500</v>
       </c>
       <c r="B41" t="s">
-        <v>21</v>
+        <v>182</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F41">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
-        <v>9300</v>
+        <v>3700</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" t="s">
-        <v>23</v>
+        <v>182</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F42">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
-        <v>11600</v>
+        <v>3900</v>
       </c>
       <c r="B43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -3961,61 +4122,119 @@
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>186</v>
-      </c>
-      <c r="G43" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F43">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
-        <v>14600</v>
+        <v>2400</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>187</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D44">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+      <c r="F44">
+        <f>115+170</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <v>15800</v>
+        <v>4500</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>187</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>190</v>
-      </c>
-      <c r="E46" t="s">
-        <v>191</v>
+        <v>31</v>
+      </c>
+      <c r="F45">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G8" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G45">
-      <sortCondition ref="A1:A8"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G46">
+      <sortCondition ref="B1:B8"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9365FEE2-AEDE-4E3A-A60D-3085849F37AC}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.06640625" style="5"/>
+    <col min="2" max="2" width="16.19921875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="21.53125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.06640625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="5">
+        <v>5801</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[5801 '22] Add to git
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E463307-6F9D-4AE6-95A1-456C042162D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28EFC20-BA94-4986-90DF-EAC2881E7491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5790" yWindow="2348" windowWidth="14400" windowHeight="7485" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5790" yWindow="2348" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -360,7 +360,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="201">
   <si>
     <t>Treinserie</t>
   </si>
@@ -957,11 +957,22 @@
     <t>- Hfdm MDWVZ</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
     <t>Hfd:
-- asdas</t>
-  </si>
-  <si>
-    <t>?</t>
+- 4640
+- 73140 (Hfdo212)
+Hfd-Shl:
+- 4340 (Hfdo213)
+- 9100/9300 niet ivm tunnel
+- 3240 niet ivm tunnel
+- 3341
+Shl:
+- 1040</t>
   </si>
 </sst>
 </file>
@@ -3252,9 +3263,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3293,184 +3304,178 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>1600</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2">
-        <f>2*85</f>
-        <v>170</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>11600</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>186</v>
-      </c>
-      <c r="F3">
-        <f>2*85</f>
-        <v>170</v>
-      </c>
-      <c r="G3" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>9100</v>
+        <v>500</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <f>110+85</f>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>140</v>
+        <v>600</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="F5">
+        <f>110+85</f>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <f>110+85</f>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>2600</v>
+        <v>800</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>182</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F7">
-        <f>2*110</f>
-        <v>220</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8">
-        <f>110+85</f>
-        <v>195</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9">
-        <f>110+85</f>
-        <v>195</v>
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>1500</v>
+        <v>1100</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>183</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10">
-        <f>110+85</f>
-        <v>195</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -3485,34 +3490,37 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>1800</v>
+        <v>1600</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>184</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>186</v>
       </c>
       <c r="F12">
-        <f>110+85</f>
-        <v>195</v>
+        <f>2*85</f>
+        <v>170</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
-        <v>2800</v>
+        <v>1800</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -3527,283 +3535,293 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>1100</v>
+        <v>2100</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="F14">
+        <f>115+170</f>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
-        <v>9200</v>
+        <v>2200</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>182</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <f>115+170</f>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
-        <v>900</v>
+        <v>2400</v>
       </c>
       <c r="B16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16">
+        <f>115+170</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>2600</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17">
+        <f>2*110</f>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>2800</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
         <v>7</v>
       </c>
-      <c r="C16">
-        <v>7</v>
-      </c>
-      <c r="D16">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>1000</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
-        <v>7</v>
-      </c>
-      <c r="D17">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>7400</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>12</v>
-      </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F18">
-        <f>2*105</f>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+        <f>110+85</f>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>4000</v>
+        <v>2900</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>182</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>3000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
         <v>10</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20">
+        <f>115+170</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>3100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>3200</v>
+      </c>
+      <c r="B22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>3300</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23">
+        <f>2*80</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>3500</v>
+      </c>
+      <c r="B24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>3700</v>
+      </c>
+      <c r="B25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>3900</v>
+      </c>
+      <c r="B26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>4000</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
         <v>35</v>
       </c>
-      <c r="F19">
+      <c r="F27">
         <f>105+75</f>
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>4800</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20">
-        <v>6</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20">
-        <f>105+75</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>5400</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21">
-        <f>105+75</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>5700</v>
-      </c>
-      <c r="B22" t="s">
-        <v>135</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22">
-        <f>2*80</f>
-        <v>160</v>
-      </c>
-      <c r="G22" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>7700</v>
-      </c>
-      <c r="B23" t="s">
-        <v>189</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
-      <c r="D23">
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23">
-        <f>2*105</f>
-        <v>210</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>14600</v>
-      </c>
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24">
-        <f>2*80+65</f>
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>4600</v>
-      </c>
-      <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25">
-        <v>7</v>
-      </c>
-      <c r="D25">
-        <v>11</v>
-      </c>
-      <c r="E25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25">
-        <f>2*80+65</f>
-        <v>225</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>3300</v>
-      </c>
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26">
-        <f>2*80</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>5100</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27">
-        <v>7</v>
-      </c>
-      <c r="D27">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27">
-        <f>2*80</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>4300</v>
       </c>
@@ -3824,355 +3842,351 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
+        <v>4500</v>
+      </c>
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>4600</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30">
+        <f>2*80+65</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>4800</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31">
+        <f>105+75</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32">
         <v>5000</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>16</v>
       </c>
-      <c r="C29">
-        <v>6</v>
-      </c>
-      <c r="D29">
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
         <v>7</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E32" t="s">
         <v>25</v>
       </c>
-      <c r="F29">
+      <c r="F32">
         <f>65+80</f>
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>5100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <f>2*80</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>5200</v>
+      </c>
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34">
+        <f>2*80</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>5400</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35">
+        <f>105+75</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>5700</v>
+      </c>
+      <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36">
+        <f>2*80</f>
+        <v>160</v>
+      </c>
+      <c r="G36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37">
         <v>5800</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B37" t="s">
         <v>16</v>
       </c>
-      <c r="C30">
-        <v>6</v>
-      </c>
-      <c r="D30">
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
         <v>7</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E37" t="s">
         <v>25</v>
       </c>
-      <c r="F30">
+      <c r="F37">
         <f>65+80</f>
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A31">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>7400</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38">
+        <f>2*105</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>7700</v>
+      </c>
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39">
+        <f>2*105</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>9100</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>9200</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>9300</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>11600</v>
+      </c>
+      <c r="B43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>186</v>
+      </c>
+      <c r="F43">
+        <f>2*85</f>
+        <v>170</v>
+      </c>
+      <c r="G43" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>14600</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44">
+        <f>2*80+65</f>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45">
         <v>15800</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B45" t="s">
         <v>16</v>
       </c>
-      <c r="C31">
-        <v>6</v>
-      </c>
-      <c r="D31">
+      <c r="C45">
+        <v>6</v>
+      </c>
+      <c r="D45">
         <v>7</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E45" t="s">
         <v>25</v>
       </c>
-      <c r="F31">
+      <c r="F45">
         <f>65+80</f>
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32">
-        <v>5200</v>
-      </c>
-      <c r="B32" t="s">
-        <v>188</v>
-      </c>
-      <c r="C32">
-        <v>7</v>
-      </c>
-      <c r="D32">
-        <v>8</v>
-      </c>
-      <c r="E32" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32">
-        <f>2*80</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <v>9300</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <v>2100</v>
-      </c>
-      <c r="B34" t="s">
-        <v>182</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-      <c r="D34">
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34">
-        <f>115+170</f>
-        <v>285</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35">
-        <v>2200</v>
-      </c>
-      <c r="B35" t="s">
-        <v>182</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-      <c r="D35">
-        <v>10</v>
-      </c>
-      <c r="E35" t="s">
-        <v>31</v>
-      </c>
-      <c r="F35">
-        <f>115+170</f>
-        <v>285</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>3000</v>
-      </c>
-      <c r="B36" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36">
-        <v>10</v>
-      </c>
-      <c r="E36" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36">
-        <f>115+170</f>
-        <v>285</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37">
-        <v>800</v>
-      </c>
-      <c r="B37" t="s">
-        <v>182</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <v>2900</v>
-      </c>
-      <c r="B38" t="s">
-        <v>182</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38">
-        <v>6</v>
-      </c>
-      <c r="E38" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39">
-        <v>3100</v>
-      </c>
-      <c r="B39" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F39">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40">
-        <v>3200</v>
-      </c>
-      <c r="B40" t="s">
-        <v>182</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40">
-        <v>6</v>
-      </c>
-      <c r="E40" t="s">
-        <v>31</v>
-      </c>
-      <c r="F40">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>3500</v>
-      </c>
-      <c r="B41" t="s">
-        <v>182</v>
-      </c>
-      <c r="C41">
-        <v>4</v>
-      </c>
-      <c r="D41">
-        <v>6</v>
-      </c>
-      <c r="E41" t="s">
-        <v>31</v>
-      </c>
-      <c r="F41">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42">
-        <v>3700</v>
-      </c>
-      <c r="B42" t="s">
-        <v>182</v>
-      </c>
-      <c r="C42">
-        <v>4</v>
-      </c>
-      <c r="D42">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F42">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>3900</v>
-      </c>
-      <c r="B43" t="s">
-        <v>182</v>
-      </c>
-      <c r="C43">
-        <v>4</v>
-      </c>
-      <c r="D43">
-        <v>6</v>
-      </c>
-      <c r="E43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F43">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>2400</v>
-      </c>
-      <c r="B44" t="s">
-        <v>187</v>
-      </c>
-      <c r="C44">
-        <v>4</v>
-      </c>
-      <c r="D44">
-        <v>10</v>
-      </c>
-      <c r="E44" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44">
-        <f>115+170</f>
-        <v>285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45">
-        <v>4500</v>
-      </c>
-      <c r="B45" t="s">
-        <v>187</v>
-      </c>
-      <c r="C45">
-        <v>4</v>
-      </c>
-      <c r="D45">
-        <v>6</v>
-      </c>
-      <c r="E45" t="s">
-        <v>31</v>
-      </c>
-      <c r="F45">
-        <v>170</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:G8" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G46">
-      <sortCondition ref="B1:B8"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G45">
+      <sortCondition ref="A1:A8"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4184,7 +4198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9365FEE2-AEDE-4E3A-A60D-3085849F37AC}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4223,7 +4237,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="156.75" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>5801</v>
       </c>
@@ -4231,7 +4245,7 @@
         <v>197</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[HSL 5801 '22] AI traffic
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28EFC20-BA94-4986-90DF-EAC2881E7491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCFEABA-AFE1-4CA9-9917-CDD93A0B96C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5790" yWindow="2348" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2348" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="ZWNL Goederenverbindingen" sheetId="4" r:id="rId3"/>
     <sheet name="ZvNL Treinseries" sheetId="3" r:id="rId4"/>
     <sheet name="HSL Treinseries" sheetId="5" r:id="rId5"/>
-    <sheet name="HSL Scenarios" sheetId="6" r:id="rId6"/>
+    <sheet name="HSL Scenarios" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
@@ -360,7 +360,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="209">
   <si>
     <t>Treinserie</t>
   </si>
@@ -942,9 +942,6 @@
     <t>AI</t>
   </si>
   <si>
-    <t>Statisch</t>
-  </si>
-  <si>
     <t>Treinen vóór speler</t>
   </si>
   <si>
@@ -961,18 +958,65 @@
   </si>
   <si>
     <t>0.05</t>
+  </si>
+  <si>
+    <t>Asdl-Ass:
+- 4640
+- 9340</t>
+  </si>
+  <si>
+    <t>Shl-Asdl:
+- 2441
+- 5740
+- 5840
+- 940</t>
+  </si>
+  <si>
+    <t>Shl:
+- 1040
+- 3540
+- 9240</t>
   </si>
   <si>
     <t>Hfd:
 - 4640
-- 73140 (Hfdo212)
-Hfd-Shl:
+- 73140 (Hfdo212)</t>
+  </si>
+  <si>
+    <t>Hfd-Shl:
 - 4340 (Hfdo213)
 - 9100/9300 niet ivm tunnel
 - 3240 niet ivm tunnel
-- 3341
-Shl:
-- 1040</t>
+- 3341</t>
+  </si>
+  <si>
+    <t>Ass-Asd:
+- 7440
+- 1040
+- 4841 Asd1
+- 9240 Asd15a
+- 840 Asd8a</t>
+  </si>
+  <si>
+    <t>Asd:
+- 104/124/222 7b
+- 940/941 14a
+- 1539/2640 11b
+- 2240/2241 2a
+- 15840 14b
+- 105 7a
+- 145/245 10a</t>
+  </si>
+  <si>
+    <t>Opstel</t>
+  </si>
+  <si>
+    <t>- Asd
+- Aswplz</t>
+  </si>
+  <si>
+    <t>- 941 Shl2-Ass
+- 1641/11643 Shl3-Asra</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1074,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1061,6 +1105,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1074,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1103,8 +1153,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3265,7 +3327,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3447,7 +3509,7 @@
         <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -4083,10 +4145,10 @@
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
@@ -4195,58 +4257,107 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9365FEE2-AEDE-4E3A-A60D-3085849F37AC}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F87682-53E5-48AC-886B-E08EE2D8C03E}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="5"/>
-    <col min="2" max="2" width="16.19921875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="21.53125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16" style="5" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.19921875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.06640625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="5"/>
+    <col min="1" max="1" width="18.19921875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.06640625" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="9.06640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="16">
+        <v>5801</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B2" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="B3" s="19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="16"/>
+      <c r="B4" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="16"/>
+      <c r="B5" s="19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="16"/>
+      <c r="B6" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="16"/>
+      <c r="B7" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="16"/>
+      <c r="B8" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+      <c r="A9" s="16"/>
+      <c r="B9" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B11" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="16"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="5">
-        <v>5801</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="B13" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5871] Add to git
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCFEABA-AFE1-4CA9-9917-CDD93A0B96C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB206668-65BB-481F-99DD-962C094A022D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2348" windowWidth="14400" windowHeight="7485" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2348" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
     <sheet name="ZWNL Treinseries" sheetId="1" r:id="rId2"/>
     <sheet name="ZWNL Goederenverbindingen" sheetId="4" r:id="rId3"/>
     <sheet name="ZvNL Treinseries" sheetId="3" r:id="rId4"/>
-    <sheet name="HSL Treinseries" sheetId="5" r:id="rId5"/>
-    <sheet name="HSL Scenarios" sheetId="7" r:id="rId6"/>
+    <sheet name="HSL Scenarios" sheetId="7" r:id="rId5"/>
+    <sheet name="HSL Treinseries" sheetId="5" r:id="rId6"/>
+    <sheet name="HSL Standard Scenarios" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZvNL Treinseries'!$A$1:$F$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL Goederenverbindingen'!$A$20:$E$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ZWNL Treinseries'!$A$1:$F$30</definedName>
@@ -360,7 +361,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="218">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1017,6 +1018,42 @@
   <si>
     <t>- 941 Shl2-Ass
 - 1641/11643 Shl3-Asra</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Timetable</t>
+  </si>
+  <si>
+    <t>- Hfdm</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>5871 Summer Clear</t>
+  </si>
+  <si>
+    <t>Hfdm:
+- 71600 (Hfdo212)
+- 700</t>
+  </si>
+  <si>
+    <t>- 901 Hfd-Asd14a
+- 71601 Hfdo-Asdz</t>
+  </si>
+  <si>
+    <t>Hfd:
+- 4600 Shl-Ledn
+- 73100 Shl-Hfdo213</t>
+  </si>
+  <si>
+    <t>Hfd-Shl:
+- 4300 Shl-Hfdo
+- 9101 Shl-HSL
+- 3200 Shl-Ledn
+- 3300 Shl-Ledn</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1167,6 +1204,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3322,12 +3365,120 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F87682-53E5-48AC-886B-E08EE2D8C03E}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.19921875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.06640625" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="9.06640625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="16">
+        <v>5801</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="16"/>
+      <c r="B4" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="16"/>
+      <c r="B5" s="19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="16"/>
+      <c r="B6" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="16"/>
+      <c r="B7" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="16"/>
+      <c r="B8" s="19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+      <c r="A9" s="16"/>
+      <c r="B9" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="16"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4256,108 +4407,85 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F87682-53E5-48AC-886B-E08EE2D8C03E}">
-  <dimension ref="A1:B13"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB0742C-EC66-4F99-8292-0EC67D49CAE5}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.19921875" style="17" customWidth="1"/>
-    <col min="2" max="2" width="20.06640625" style="17" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="17"/>
+    <col min="1" max="1" width="18.1328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9.06640625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="16">
-        <v>5801</v>
+      <c r="B1" s="5" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>196</v>
+      <c r="A2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="16"/>
-      <c r="B4" s="19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A5" s="16"/>
-      <c r="B5" s="19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="16"/>
-      <c r="B6" s="19" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="16"/>
-      <c r="B7" s="19" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="16"/>
-      <c r="B8" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A9" s="16"/>
-      <c r="B9" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="16" t="s">
+      <c r="B3" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B4" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B5" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>207</v>
+      <c r="B10" s="21" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>208</v>
+      <c r="B11" s="22" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B12" s="16"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="16" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B13" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[5871] Verander rijweg om sein Shl RA te fixen
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB206668-65BB-481F-99DD-962C094A022D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6194B2E-A57C-41E4-B00C-D1E07AA548D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2348" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6495" yWindow="3067" windowWidth="14400" windowHeight="7486" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="HSL Scenarios" sheetId="7" r:id="rId5"/>
     <sheet name="HSL Treinseries" sheetId="5" r:id="rId6"/>
     <sheet name="HSL Standard Scenarios" sheetId="8" r:id="rId7"/>
+    <sheet name="HSL Opmerkingen" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
@@ -361,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="219">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1054,6 +1055,9 @@
 - 9101 Shl-HSL
 - 3200 Shl-Ledn
 - 3300 Shl-Ledn</t>
+  </si>
+  <si>
+    <t>Schiphol uitrijsein op RA wordt niet goed afgereden, hier geen AI treinen vóór speler!</t>
   </si>
 </sst>
 </file>
@@ -4411,7 +4415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB0742C-EC66-4F99-8292-0EC67D49CAE5}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4490,4 +4494,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63515A09-7DDE-4638-8E31-255375D1CA8A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cargospots 2022 t/m maart
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EB694D-5457-46C9-9513-7EB9CC9217E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C4B4F6-1127-4EEB-A3C9-82DA75156CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4568" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6562" yWindow="4050" windowWidth="14400" windowHeight="7485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
-    <sheet name="ZWNL Treinseries" sheetId="1" r:id="rId2"/>
-    <sheet name="ZWNL Goederenverbindingen" sheetId="4" r:id="rId3"/>
-    <sheet name="ZvNL Treinseries" sheetId="3" r:id="rId4"/>
-    <sheet name="HSL Scenarios" sheetId="7" r:id="rId5"/>
-    <sheet name="HSL Treinseries" sheetId="5" r:id="rId6"/>
-    <sheet name="HSL Standard Scenarios" sheetId="8" r:id="rId7"/>
-    <sheet name="HSL Opmerkingen" sheetId="9" r:id="rId8"/>
+    <sheet name="Goederenspots" sheetId="10" r:id="rId2"/>
+    <sheet name="ZWNL Treinseries" sheetId="1" r:id="rId3"/>
+    <sheet name="ZWNL Goederenverbindingen" sheetId="4" r:id="rId4"/>
+    <sheet name="ZvNL Treinseries" sheetId="3" r:id="rId5"/>
+    <sheet name="HSL Scenarios" sheetId="7" r:id="rId6"/>
+    <sheet name="HSL Treinseries" sheetId="5" r:id="rId7"/>
+    <sheet name="HSL Standard Scenarios" sheetId="8" r:id="rId8"/>
+    <sheet name="HSL Opmerkingen" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZvNL Treinseries'!$A$1:$F$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL Goederenverbindingen'!$A$20:$E$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ZWNL Treinseries'!$A$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ZvNL Treinseries'!$A$1:$F$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL Goederenverbindingen'!$A$20:$E$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL Treinseries'!$A$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -362,7 +363,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="322">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1143,12 +1144,288 @@
     <t>Toegevoegd
 - 120 Asd2b</t>
   </si>
+  <si>
+    <t>Video URL</t>
+  </si>
+  <si>
+    <t>Locatie</t>
+  </si>
+  <si>
+    <t>Richting</t>
+  </si>
+  <si>
+    <t>Tijd</t>
+  </si>
+  <si>
+    <t>Opmerkingen</t>
+  </si>
+  <si>
+    <t>Rsd</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Stilstaand, 186+Uacns</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LKsnlTb3KsM?t=68</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LKsnlTb3KsM?t=1103</t>
+  </si>
+  <si>
+    <t>Bda</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LKsnlTb3KsM?t=1315</t>
+  </si>
+  <si>
+    <t>Zelfde as 08:42. Mogelijk vertraagd.</t>
+  </si>
+  <si>
+    <t>2x189DBC+F. Mogelijk vertraagd.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QcaplDpuBgw?t=84</t>
+  </si>
+  <si>
+    <t>Wd</t>
+  </si>
+  <si>
+    <t>https://youtu.be/QcaplDpuBgw?t=316</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ijVJM8_I2QU?t=226</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ijVJM8_I2QU?t=278</t>
+  </si>
+  <si>
+    <t>https://youtu.be/F3i4iIlBxUE?t=231</t>
+  </si>
+  <si>
+    <t>Tbr</t>
+  </si>
+  <si>
+    <t>https://youtu.be/my9a52XBmVM?t=252</t>
+  </si>
+  <si>
+    <t>Zlw</t>
+  </si>
+  <si>
+    <t>https://youtu.be/my9a52XBmVM?t=303</t>
+  </si>
+  <si>
+    <t>https://youtu.be/my9a52XBmVM?t=335</t>
+  </si>
+  <si>
+    <t>Ddr</t>
+  </si>
+  <si>
+    <t>Uit Bd</t>
+  </si>
+  <si>
+    <t>https://youtu.be/my9a52XBmVM?t=400</t>
+  </si>
+  <si>
+    <t>https://youtu.be/my9a52XBmVM?t=451</t>
+  </si>
+  <si>
+    <t>https://youtu.be/my9a52XBmVM?t=502</t>
+  </si>
+  <si>
+    <t>https://youtu.be/knBd-kiZZg4?t=144</t>
+  </si>
+  <si>
+    <t>Ehs</t>
+  </si>
+  <si>
+    <t>Ehv</t>
+  </si>
+  <si>
+    <t>https://youtu.be/knBd-kiZZg4?t=423</t>
+  </si>
+  <si>
+    <t>Btl</t>
+  </si>
+  <si>
+    <t>Buitenspoor</t>
+  </si>
+  <si>
+    <t>https://youtu.be/gPwr4c_5HC8?t=64</t>
+  </si>
+  <si>
+    <t>Mas</t>
+  </si>
+  <si>
+    <t>Binnenspoor</t>
+  </si>
+  <si>
+    <t>https://youtu.be/1XBpSkOoo1I?t=374</t>
+  </si>
+  <si>
+    <t>https://youtu.be/5FwB7lj87bs?t=113</t>
+  </si>
+  <si>
+    <t>Htnc</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fAURKIs8WM8?t=234</t>
+  </si>
+  <si>
+    <t>Zwd</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>https://youtu.be/kN323NbK6EQ?t=123</t>
+  </si>
+  <si>
+    <t>Tbu</t>
+  </si>
+  <si>
+    <t>Tb</t>
+  </si>
+  <si>
+    <t>https://youtu.be/nuLM1uP7NnQ?t=612</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=88</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=176</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=305</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=354</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=386</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=436</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=515</t>
+  </si>
+  <si>
+    <t>Spoor 3</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=596</t>
+  </si>
+  <si>
+    <t>Spoor 2</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=646</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=721</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LVTLIsVrSPE?t=776</t>
+  </si>
+  <si>
+    <t>https://youtu.be/RUSYQ8XDz3I?t=1060</t>
+  </si>
+  <si>
+    <t>Ledn</t>
+  </si>
+  <si>
+    <t>Spoor 10</t>
+  </si>
+  <si>
+    <t>https://youtu.be/KVx4aXPJIA4?t=9</t>
+  </si>
+  <si>
+    <t>Uit Ht</t>
+  </si>
+  <si>
+    <t>https://youtu.be/KVx4aXPJIA4?t=1823</t>
+  </si>
+  <si>
+    <t>Uit Tb</t>
+  </si>
+  <si>
+    <t>https://youtu.be/TZw32Ih6u54?t=179</t>
+  </si>
+  <si>
+    <t>https://youtu.be/8Rj7hH8cDmQ?t=18</t>
+  </si>
+  <si>
+    <t>https://youtu.be/K0ikFyFuCjA?t=7</t>
+  </si>
+  <si>
+    <t>Ot</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0ootBb1r9nQ?t=37</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0ootBb1r9nQ?t=61</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0ootBb1r9nQ?t=110</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0ootBb1r9nQ?t=163</t>
+  </si>
+  <si>
+    <t>https://youtu.be/0ootBb1r9nQ?t=234</t>
+  </si>
+  <si>
+    <t>Nr</t>
+  </si>
+  <si>
+    <t>https://youtu.be/NsP4el52oCg?t=15</t>
+  </si>
+  <si>
+    <t>https://youtu.be/FSY4H5LixBo?t=131</t>
+  </si>
+  <si>
+    <t>Nmgo</t>
+  </si>
+  <si>
+    <t>Ht</t>
+  </si>
+  <si>
+    <t>https://youtu.be/EtmCoFMUjnY?t=283</t>
+  </si>
+  <si>
+    <t>Ost</t>
+  </si>
+  <si>
+    <t>Dv</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fvpAiMD3I_c?t=177</t>
+  </si>
+  <si>
+    <t>Dvc</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fvpAiMD3I_c?t=232</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ZBer_xP5xdA?t=18</t>
+  </si>
+  <si>
+    <t>Gz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1197,6 +1474,25 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1249,7 +1545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1308,6 +1604,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2067,6 +2366,981 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B64A02-8D48-40E3-B121-B38BAF0C0B33}">
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="30.06640625" style="26" customWidth="1"/>
+    <col min="3" max="5" width="9.06640625" style="26"/>
+    <col min="6" max="6" width="35.73046875" style="26" customWidth="1"/>
+    <col min="7" max="16384" width="9.06640625" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="26">
+        <v>100</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="E2" s="28">
+        <v>22</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="26">
+        <v>200</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" s="28">
+        <v>42</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="26">
+        <v>300</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="28">
+        <v>45</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="26">
+        <v>400</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" s="26">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="26">
+        <v>500</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="E6" s="26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="26">
+        <v>600</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="26">
+        <v>700</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="E8" s="26">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="26">
+        <v>800</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="26">
+        <v>900</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="26">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="26">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="26">
+        <v>1100</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="26">
+        <v>1</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="26">
+        <v>1200</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="26">
+        <v>1300</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="E14" s="26">
+        <v>25</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="26">
+        <v>1400</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="26">
+        <v>1500</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" s="26">
+        <v>12</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="26">
+        <v>1600</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" s="26">
+        <v>17</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="26">
+        <v>1700</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="E18" s="26">
+        <v>30</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="26">
+        <v>1800</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="E19" s="26">
+        <v>3</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="26">
+        <v>1900</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="E20" s="26">
+        <v>43</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="26">
+        <v>2000</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="E21" s="26">
+        <v>36</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="26">
+        <v>2100</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E22" s="26">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="26">
+        <v>2200</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="26">
+        <v>49</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="26">
+        <v>2300</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="26">
+        <v>12</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="26">
+        <v>2400</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="26">
+        <v>44</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="26">
+        <v>2500</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="26">
+        <v>15</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="26">
+        <v>2600</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E27" s="26">
+        <v>21</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="26">
+        <v>2700</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="26">
+        <v>33</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="26">
+        <v>2800</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="26">
+        <v>41</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="26">
+        <v>2900</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="26">
+        <v>2</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="26">
+        <v>3000</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="26">
+        <v>19</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="26">
+        <v>3100</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="26">
+        <v>31</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="26">
+        <v>3200</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E33" s="26">
+        <v>42</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="26">
+        <v>3300</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E34" s="26">
+        <v>0</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="26">
+        <v>3400</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="E35" s="26">
+        <v>1</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="26">
+        <v>3500</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E36" s="26">
+        <v>28</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="26">
+        <v>3600</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E37" s="26">
+        <v>58</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="26">
+        <v>3700</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E38" s="26">
+        <v>30</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="26">
+        <v>3800</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E39" s="26">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="26">
+        <v>3900</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E40" s="26">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="26">
+        <v>4000</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="E41" s="26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="26">
+        <v>4100</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E42" s="26">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="26">
+        <v>4200</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E43" s="26">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="26">
+        <v>4300</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>307</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="E44" s="26">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="26">
+        <v>4400</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E45" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="26">
+        <v>4500</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E46" s="26">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="26">
+        <v>4600</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="E47" s="26">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="26">
+        <v>4700</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E48" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49" s="26">
+        <v>4800</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E49" s="26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50" s="26">
+        <v>4900</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E50" s="26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" s="26">
+        <v>5000</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E51" s="26">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
@@ -2517,7 +3791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA394F4-D495-45BA-A765-8FE37C144B84}">
   <dimension ref="A1:I30"/>
   <sheetViews>
@@ -2931,7 +4205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35417EC1-5320-4F84-8CF8-205F491D5996}">
   <dimension ref="A1:F34"/>
   <sheetViews>
@@ -3461,7 +4735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F87682-53E5-48AC-886B-E08EE2D8C03E}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -3569,7 +4843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
   <dimension ref="A1:G45"/>
   <sheetViews>
@@ -4504,11 +5778,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB0742C-EC66-4F99-8292-0EC67D49CAE5}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -4649,7 +5923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63515A09-7DDE-4638-8E31-255375D1CA8A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Drgl bestanden voor cargospots
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C4B4F6-1127-4EEB-A3C9-82DA75156CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDE6C30-0CE0-4541-AB3E-52B31693AE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6562" yWindow="4050" windowWidth="14400" windowHeight="7485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <sheet name="HSL Opmerkingen" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goederenspots!$A$1:$F$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ZvNL Treinseries'!$A$1:$F$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL Goederenverbindingen'!$A$20:$E$30</definedName>
@@ -1425,7 +1426,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1494,6 +1495,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1545,7 +1553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1607,6 +1615,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2369,8 +2380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B64A02-8D48-40E3-B121-B38BAF0C0B33}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2403,481 +2414,472 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="26">
-        <v>100</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="E2" s="28">
-        <v>22</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>237</v>
+      <c r="A2" s="29">
+        <v>200</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="E2" s="30">
+        <v>42</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="26">
-        <v>200</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="A3" s="29">
+        <v>300</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="30">
+        <v>45</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="31">
+        <v>3500</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="26">
+        <v>28</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="31">
+        <v>3700</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" s="26">
+        <v>30</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="31">
+        <v>3800</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E6" s="26">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="31">
+        <v>3600</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E7" s="26">
+        <v>58</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="31">
+        <v>4800</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E8" s="26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="31">
+        <v>4900</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E9" s="26">
         <v>42</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="26">
-        <v>300</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>242</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="E4" s="28">
-        <v>45</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="26">
-        <v>400</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="E5" s="26">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="26">
-        <v>500</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>247</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="E6" s="26">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="26">
-        <v>600</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="E7" s="26">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="26">
-        <v>700</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>241</v>
-      </c>
-      <c r="E8" s="26">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="26">
-        <v>800</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="E9" s="26">
-        <v>10</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="26">
-        <v>900</v>
+      <c r="A10" s="31">
+        <v>1800</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>153</v>
+        <v>265</v>
       </c>
       <c r="E10" s="26">
-        <v>28</v>
+        <v>3</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="26">
-        <v>1000</v>
+      <c r="A11" s="31">
+        <v>1500</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="E11" s="26">
-        <v>51</v>
+        <v>12</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="26">
-        <v>1100</v>
+      <c r="A12" s="31">
+        <v>1600</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="E12" s="26">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="26">
-        <v>1200</v>
+        <v>5000</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>258</v>
+        <v>320</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>253</v>
+        <v>321</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>153</v>
+        <v>278</v>
       </c>
       <c r="E13" s="26">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="26">
-        <v>1300</v>
+        <v>1900</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="E14" s="26">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="26">
-        <v>1400</v>
+        <v>3400</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>260</v>
+        <v>293</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>253</v>
+        <v>294</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>153</v>
+        <v>275</v>
       </c>
       <c r="E15" s="26">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="26">
-        <v>1500</v>
+        <v>1700</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="E16" s="26">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="26">
-        <v>1600</v>
+        <v>4600</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>264</v>
+        <v>311</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>262</v>
+        <v>312</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>265</v>
+        <v>313</v>
       </c>
       <c r="E17" s="26">
-        <v>17</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>266</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="26">
-        <v>1700</v>
+        <v>4700</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>267</v>
+        <v>314</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>268</v>
+        <v>315</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>236</v>
+        <v>316</v>
       </c>
       <c r="E18" s="26">
-        <v>30</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>269</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="26">
-        <v>1800</v>
+      <c r="A19" s="31">
+        <v>4400</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>270</v>
+        <v>308</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>262</v>
+        <v>303</v>
       </c>
       <c r="D19" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E19" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="31">
+        <v>4000</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D20" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="E19" s="26">
-        <v>3</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="26">
-        <v>1900</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>272</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>236</v>
-      </c>
       <c r="E20" s="26">
-        <v>43</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>266</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="26">
-        <v>2000</v>
+      <c r="A21" s="31">
+        <v>4300</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>274</v>
+        <v>303</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="E21" s="26">
-        <v>36</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>266</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="26">
-        <v>2100</v>
+      <c r="A22" s="31">
+        <v>4200</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>276</v>
+        <v>306</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>278</v>
       </c>
       <c r="E22" s="26">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="26">
-        <v>2200</v>
+      <c r="A23" s="31">
+        <v>3900</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="C23" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="D23" s="26" t="s">
-        <v>153</v>
-      </c>
       <c r="E23" s="26">
-        <v>49</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>289</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="26">
-        <v>2300</v>
+      <c r="A24" s="31">
+        <v>4500</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>280</v>
+        <v>310</v>
       </c>
       <c r="C24" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D24" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="D24" s="26" t="s">
-        <v>153</v>
-      </c>
       <c r="E24" s="26">
-        <v>12</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>289</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="26">
-        <v>2400</v>
+      <c r="A25" s="31">
+        <v>4100</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="C25" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="D25" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="D25" s="26" t="s">
-        <v>153</v>
-      </c>
       <c r="E25" s="26">
-        <v>44</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>289</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="26">
-        <v>2500</v>
+      <c r="A26" s="31">
+        <v>100</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>282</v>
+        <v>238</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>278</v>
+        <v>235</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="E26" s="26">
-        <v>15</v>
+        <v>236</v>
+      </c>
+      <c r="E26" s="28">
+        <v>22</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>289</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="26">
-        <v>2600</v>
+      <c r="A27" s="31">
+        <v>3300</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>278</v>
@@ -2886,18 +2888,18 @@
         <v>153</v>
       </c>
       <c r="E27" s="26">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F27" s="26" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="26">
-        <v>2700</v>
+      <c r="A28" s="31">
+        <v>2900</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>278</v>
@@ -2906,18 +2908,18 @@
         <v>153</v>
       </c>
       <c r="E28" s="26">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="26">
-        <v>2800</v>
+      <c r="A29" s="31">
+        <v>2300</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>278</v>
@@ -2926,18 +2928,18 @@
         <v>153</v>
       </c>
       <c r="E29" s="26">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="F29" s="26" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="26">
-        <v>2900</v>
+      <c r="A30" s="31">
+        <v>2500</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>278</v>
@@ -2946,14 +2948,14 @@
         <v>153</v>
       </c>
       <c r="E30" s="26">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="26">
+      <c r="A31" s="31">
         <v>3000</v>
       </c>
       <c r="B31" s="26" t="s">
@@ -2973,11 +2975,11 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="26">
-        <v>3100</v>
+      <c r="A32" s="31">
+        <v>2600</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>278</v>
@@ -2986,18 +2988,18 @@
         <v>153</v>
       </c>
       <c r="E32" s="26">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="26">
-        <v>3200</v>
+      <c r="A33" s="31">
+        <v>3100</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>278</v>
@@ -3006,18 +3008,18 @@
         <v>153</v>
       </c>
       <c r="E33" s="26">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F33" s="26" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="26">
-        <v>3300</v>
+      <c r="A34" s="31">
+        <v>2700</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>278</v>
@@ -3026,314 +3028,328 @@
         <v>153</v>
       </c>
       <c r="E34" s="26">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F34" s="26" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="26">
-        <v>3400</v>
+      <c r="A35" s="31">
+        <v>2800</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>275</v>
+        <v>153</v>
       </c>
       <c r="E35" s="26">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="26">
-        <v>3500</v>
+      <c r="A36" s="31">
+        <v>3200</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>263</v>
+        <v>153</v>
       </c>
       <c r="E36" s="26">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="26">
-        <v>3600</v>
+      <c r="A37" s="31">
+        <v>2400</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>263</v>
+        <v>153</v>
       </c>
       <c r="E37" s="26">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="26">
-        <v>3700</v>
+      <c r="A38" s="31">
+        <v>2200</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>263</v>
+        <v>153</v>
       </c>
       <c r="E38" s="26">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="26">
-        <v>3800</v>
+      <c r="A39" s="31">
+        <v>800</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>301</v>
+        <v>250</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>278</v>
+        <v>153</v>
       </c>
       <c r="E39" s="26">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="26">
-        <v>3900</v>
+      <c r="A40" s="31">
+        <v>2100</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>302</v>
+        <v>276</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>278</v>
       </c>
       <c r="E40" s="26">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="26">
-        <v>4000</v>
+        <v>500</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>304</v>
+        <v>247</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>303</v>
+        <v>246</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="E41" s="26">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="26">
-        <v>4100</v>
+        <v>600</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>303</v>
+        <v>246</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="E42" s="26">
-        <v>51</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="26">
-        <v>4200</v>
+        <v>400</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>306</v>
+        <v>245</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>303</v>
+        <v>246</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="E43" s="26">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="26">
-        <v>4300</v>
+        <v>700</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>307</v>
+        <v>249</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>303</v>
+        <v>246</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="E44" s="26">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="26">
-        <v>4400</v>
+      <c r="A45" s="31">
+        <v>1100</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>308</v>
+        <v>255</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="E45" s="26">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F45" s="26" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="26">
-        <v>4500</v>
+      <c r="A46" s="31">
+        <v>1200</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>310</v>
+        <v>258</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>278</v>
+        <v>153</v>
       </c>
       <c r="E46" s="26">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="26">
-        <v>4600</v>
+      <c r="A47" s="31">
+        <v>1300</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>311</v>
+        <v>259</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>312</v>
+        <v>253</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>313</v>
+        <v>256</v>
       </c>
       <c r="E47" s="26">
-        <v>47</v>
+        <v>25</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="26">
-        <v>4700</v>
+      <c r="A48" s="31">
+        <v>900</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>314</v>
+        <v>252</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>315</v>
+        <v>253</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>316</v>
+        <v>153</v>
       </c>
       <c r="E48" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A49" s="26">
-        <v>4800</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="31">
+        <v>1400</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>317</v>
+        <v>260</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>318</v>
+        <v>253</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>316</v>
+        <v>153</v>
       </c>
       <c r="E49" s="26">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A50" s="26">
-        <v>4900</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="31">
+        <v>1000</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>319</v>
+        <v>254</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>318</v>
+        <v>253</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>316</v>
+        <v>153</v>
       </c>
       <c r="E50" s="26">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A51" s="26">
-        <v>5000</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="31">
+        <v>2000</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>320</v>
+        <v>273</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>321</v>
+        <v>274</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E51" s="26">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="F51" s="26" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F51" xr:uid="{27B64A02-8D48-40E3-B121-B38BAF0C0B33}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F51">
+      <sortCondition ref="C1:C51"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Cargotijden rail magazine 391-392
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4D4382-D7B2-420E-925E-7B5234229F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13770E62-6F7F-4FD5-A739-8BA9CBF29AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6562" yWindow="4050" windowWidth="14400" windowHeight="7485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6503" yWindow="7462" windowWidth="14401" windowHeight="7485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -364,7 +364,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="347">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1421,12 +1421,99 @@
   <si>
     <t>Gz</t>
   </si>
+  <si>
+    <t>RM392 p17</t>
+  </si>
+  <si>
+    <t>Co</t>
+  </si>
+  <si>
+    <t>Zl</t>
+  </si>
+  <si>
+    <t>Amf</t>
+  </si>
+  <si>
+    <t>Wp</t>
+  </si>
+  <si>
+    <t>Aankomst</t>
+  </si>
+  <si>
+    <t>Vertrek</t>
+  </si>
+  <si>
+    <t>RM392 p18</t>
+  </si>
+  <si>
+    <t>Lis</t>
+  </si>
+  <si>
+    <t>RM392 p19</t>
+  </si>
+  <si>
+    <t>Vdm</t>
+  </si>
+  <si>
+    <t>Gn</t>
+  </si>
+  <si>
+    <t>Onn</t>
+  </si>
+  <si>
+    <t>Hgv</t>
+  </si>
+  <si>
+    <t>Std</t>
+  </si>
+  <si>
+    <t>Dolime 47627</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aankomst. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Staaltrein 61601</t>
+    </r>
+  </si>
+  <si>
+    <t>Coevorden-shuttle 50419</t>
+  </si>
+  <si>
+    <t>Fvs</t>
+  </si>
+  <si>
+    <t>RM392 p20</t>
+  </si>
+  <si>
+    <t>Wt</t>
+  </si>
+  <si>
+    <t>Mbtwaz</t>
+  </si>
+  <si>
+    <t>Pt</t>
+  </si>
+  <si>
+    <t>uit Zl</t>
+  </si>
+  <si>
+    <t>Dolime 47628</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1502,6 +1589,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1553,7 +1647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1618,6 +1712,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2378,10 +2473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B64A02-8D48-40E3-B121-B38BAF0C0B33}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2414,31 +2509,31 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="29">
-        <v>200</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>239</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>241</v>
-      </c>
-      <c r="E2" s="30">
-        <v>42</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>244</v>
+      <c r="A2" s="31">
+        <v>100</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="E2" s="28">
+        <v>22</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="29">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C3" s="29" t="s">
         <v>240</v>
@@ -2447,439 +2542,448 @@
         <v>241</v>
       </c>
       <c r="E3" s="30">
+        <v>42</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="29">
+        <v>300</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="30">
         <v>45</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F4" s="29" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="31">
-        <v>3500</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>296</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="E4" s="26">
-        <v>28</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>297</v>
-      </c>
-    </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="31">
-        <v>3600</v>
+      <c r="A5" s="26">
+        <v>400</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>298</v>
+        <v>245</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="E5" s="26">
-        <v>58</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>299</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="31">
-        <v>3700</v>
+      <c r="A6" s="26">
+        <v>500</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>300</v>
+        <v>247</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="E6" s="26">
-        <v>30</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>299</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="31">
-        <v>3800</v>
+      <c r="A7" s="26">
+        <v>600</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>301</v>
+        <v>248</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
       <c r="E7" s="26">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="31">
-        <v>4800</v>
+      <c r="A8" s="26">
+        <v>700</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>317</v>
+        <v>249</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>318</v>
+        <v>246</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>316</v>
+        <v>241</v>
       </c>
       <c r="E8" s="26">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="31">
-        <v>4900</v>
+        <v>800</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>319</v>
+        <v>250</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>318</v>
+        <v>251</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>316</v>
+        <v>153</v>
       </c>
       <c r="E9" s="26">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="31">
-        <v>1500</v>
+        <v>900</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>263</v>
+        <v>153</v>
       </c>
       <c r="E10" s="26">
-        <v>12</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>266</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="31">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>265</v>
+        <v>153</v>
       </c>
       <c r="E11" s="26">
-        <v>17</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>266</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="31">
-        <v>1800</v>
+        <v>1100</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="C12" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="26">
+        <v>1</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="31">
+        <v>1200</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="31">
+        <v>1300</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="E14" s="26">
+        <v>25</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="31">
+        <v>1400</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="31">
+        <v>1500</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="C16" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D16" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" s="26">
+        <v>12</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="31">
+        <v>1600</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="E12" s="26">
-        <v>3</v>
-      </c>
-      <c r="F12" s="26" t="s">
+      <c r="E17" s="26">
+        <v>17</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="26">
-        <v>5000</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>320</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>321</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>278</v>
-      </c>
-      <c r="E13" s="26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="26">
-        <v>1900</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>272</v>
-      </c>
-      <c r="D14" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="E14" s="26">
-        <v>43</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="26">
-        <v>3400</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>275</v>
-      </c>
-      <c r="E15" s="26">
-        <v>1</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="26">
-        <v>1700</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>268</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="E16" s="26">
-        <v>30</v>
-      </c>
-      <c r="F16" s="26" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="26">
-        <v>4600</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="E17" s="26">
-        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="26">
-        <v>4700</v>
+        <v>1700</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>314</v>
+        <v>267</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>315</v>
+        <v>268</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>316</v>
+        <v>236</v>
       </c>
       <c r="E18" s="26">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="31">
-        <v>3900</v>
+        <v>1800</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>303</v>
+        <v>262</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="E19" s="26">
-        <v>47</v>
+        <v>3</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="31">
-        <v>4000</v>
+      <c r="A20" s="26">
+        <v>1900</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>304</v>
+        <v>271</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>303</v>
+        <v>272</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>265</v>
+        <v>236</v>
       </c>
       <c r="E20" s="26">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="31">
-        <v>4100</v>
+        <v>2000</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E21" s="26">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="31">
-        <v>4200</v>
+        <v>2100</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>278</v>
       </c>
       <c r="E22" s="26">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="31">
-        <v>4300</v>
+        <v>2200</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>265</v>
+        <v>153</v>
       </c>
       <c r="E23" s="26">
-        <v>34</v>
+        <v>49</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="31">
-        <v>4400</v>
+        <v>2300</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>278</v>
+        <v>153</v>
       </c>
       <c r="E24" s="26">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="31">
-        <v>4500</v>
+        <v>2400</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>310</v>
+        <v>281</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>278</v>
+        <v>153</v>
       </c>
       <c r="E25" s="26">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="31">
-        <v>100</v>
+        <v>2500</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>238</v>
+        <v>282</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>235</v>
+        <v>278</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="E26" s="28">
-        <v>22</v>
+        <v>153</v>
+      </c>
+      <c r="E26" s="26">
+        <v>15</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>237</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="31">
-        <v>2200</v>
+        <v>2600</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>278</v>
@@ -2888,7 +2992,7 @@
         <v>153</v>
       </c>
       <c r="E27" s="26">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F27" s="26" t="s">
         <v>289</v>
@@ -2896,10 +3000,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="31">
-        <v>2300</v>
+        <v>2700</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>278</v>
@@ -2908,7 +3012,7 @@
         <v>153</v>
       </c>
       <c r="E28" s="26">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="F28" s="26" t="s">
         <v>289</v>
@@ -2916,10 +3020,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="31">
-        <v>2400</v>
+        <v>2800</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>278</v>
@@ -2928,7 +3032,7 @@
         <v>153</v>
       </c>
       <c r="E29" s="26">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F29" s="26" t="s">
         <v>289</v>
@@ -2936,10 +3040,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="31">
-        <v>2500</v>
+        <v>2900</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>278</v>
@@ -2948,18 +3052,18 @@
         <v>153</v>
       </c>
       <c r="E30" s="26">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="31">
-        <v>2600</v>
+        <v>3000</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>278</v>
@@ -2968,7 +3072,7 @@
         <v>153</v>
       </c>
       <c r="E31" s="26">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F31" s="26" t="s">
         <v>289</v>
@@ -2976,10 +3080,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="31">
-        <v>2700</v>
+        <v>3100</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>278</v>
@@ -2988,7 +3092,7 @@
         <v>153</v>
       </c>
       <c r="E32" s="26">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F32" s="26" t="s">
         <v>289</v>
@@ -2996,10 +3100,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="31">
-        <v>2800</v>
+        <v>3200</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>278</v>
@@ -3008,7 +3112,7 @@
         <v>153</v>
       </c>
       <c r="E33" s="26">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F33" s="26" t="s">
         <v>289</v>
@@ -3016,10 +3120,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="31">
-        <v>2900</v>
+        <v>3300</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>278</v>
@@ -3028,326 +3132,837 @@
         <v>153</v>
       </c>
       <c r="E34" s="26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="31">
-        <v>3000</v>
+      <c r="A35" s="26">
+        <v>3400</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>153</v>
+        <v>275</v>
       </c>
       <c r="E35" s="26">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="31">
-        <v>3100</v>
+        <v>3500</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="E36" s="26">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="31">
-        <v>3200</v>
+        <v>3600</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="E37" s="26">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="31">
-        <v>3300</v>
+        <v>3700</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="E38" s="26">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="31">
-        <v>800</v>
+        <v>3800</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>153</v>
+        <v>278</v>
       </c>
       <c r="E39" s="26">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="31">
-        <v>2100</v>
+        <v>3900</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>276</v>
+        <v>302</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>278</v>
       </c>
       <c r="E40" s="26">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="26">
-        <v>400</v>
+      <c r="A41" s="31">
+        <v>4000</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>245</v>
+        <v>304</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="E41" s="26">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="26">
-        <v>500</v>
+      <c r="A42" s="31">
+        <v>4100</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>247</v>
+        <v>305</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>241</v>
+        <v>278</v>
       </c>
       <c r="E42" s="26">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="26">
-        <v>600</v>
+      <c r="A43" s="31">
+        <v>4200</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>248</v>
+        <v>306</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>241</v>
+        <v>278</v>
       </c>
       <c r="E43" s="26">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="26">
-        <v>700</v>
+      <c r="A44" s="31">
+        <v>4300</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="E44" s="26">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="31">
-        <v>900</v>
+        <v>4400</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>252</v>
+        <v>308</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>153</v>
+        <v>278</v>
       </c>
       <c r="E45" s="26">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="31">
-        <v>1000</v>
+        <v>4500</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>254</v>
+        <v>310</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>153</v>
+        <v>278</v>
       </c>
       <c r="E46" s="26">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="31">
-        <v>1100</v>
+      <c r="A47" s="26">
+        <v>4600</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>255</v>
+        <v>311</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>253</v>
+        <v>312</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>256</v>
+        <v>313</v>
       </c>
       <c r="E47" s="26">
-        <v>1</v>
-      </c>
-      <c r="F47" s="26" t="s">
-        <v>257</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="31">
-        <v>1200</v>
+      <c r="A48" s="26">
+        <v>4700</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>258</v>
+        <v>314</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>253</v>
+        <v>315</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>153</v>
+        <v>316</v>
       </c>
       <c r="E48" s="26">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="31">
-        <v>1300</v>
+        <v>4800</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>259</v>
+        <v>317</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>253</v>
+        <v>318</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>256</v>
+        <v>316</v>
       </c>
       <c r="E49" s="26">
-        <v>25</v>
-      </c>
-      <c r="F49" s="26" t="s">
-        <v>257</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="31">
-        <v>1400</v>
+        <v>4900</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>260</v>
+        <v>319</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>253</v>
+        <v>318</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>153</v>
+        <v>316</v>
       </c>
       <c r="E50" s="26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="26">
+        <v>5000</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E51" s="26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" s="31">
+        <v>5100</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="E52" s="26">
+        <v>7</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" s="31">
+        <v>5100</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="E53" s="26">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="31">
+        <v>5100</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="E54" s="26">
+        <v>53</v>
+      </c>
+      <c r="F54" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="31">
+        <v>5100</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="E55" s="26">
+        <v>45</v>
+      </c>
+      <c r="F55" s="26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="31">
+        <v>5100</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="E56" s="26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="31">
+        <v>5100</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E57" s="26">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="31">
+        <v>5200</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="E58" s="26">
+        <v>16</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="31">
+        <v>5200</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="E59" s="26">
+        <v>22</v>
+      </c>
+      <c r="F59" s="26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="31">
+        <v>5200</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E60" s="26">
+        <v>36</v>
+      </c>
+      <c r="F60" s="26" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="31">
+        <v>5200</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="D61" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" s="26">
+        <v>48</v>
+      </c>
+      <c r="F61" s="26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="31">
+        <v>5300</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="E62" s="26">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E63" s="26">
+        <v>54</v>
+      </c>
+      <c r="F63" s="32" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B64" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C64" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="E64" s="26">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="E65" s="26">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="E66" s="26">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="31">
-        <v>2000</v>
-      </c>
-      <c r="B51" s="26" t="s">
-        <v>273</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>274</v>
-      </c>
-      <c r="D51" s="26" t="s">
-        <v>275</v>
-      </c>
-      <c r="E51" s="26">
-        <v>36</v>
-      </c>
-      <c r="F51" s="26" t="s">
-        <v>266</v>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C67" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E67" s="26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B68" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E68" s="26">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="D69" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="E69" s="26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="E70" s="26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="31">
+        <v>5400</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="E71" s="26">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="E72" s="26">
+        <v>24</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="E73" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="E74" s="26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="D75" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="E75" s="26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="D76" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="E76" s="26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="D77" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="E77" s="26">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B78" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C78" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="E78" s="26">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B79" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C79" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="D79" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="E79" s="26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="31">
+        <v>5500</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="E80" s="26">
+        <v>35</v>
+      </c>
+      <c r="F80" s="26" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F51" xr:uid="{27B64A02-8D48-40E3-B121-B38BAF0C0B33}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F51">
-      <sortCondition ref="C1:C51"/>
+      <sortCondition ref="A1:A51"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="9" type="noConversion"/>

</xml_diff>

<commit_message>
[ZvNL] 6400 standard scenario
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13770E62-6F7F-4FD5-A739-8BA9CBF29AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F87E268-22AA-4E2C-B807-BE1D0E025DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6503" yWindow="7462" windowWidth="14401" windowHeight="7485" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6885" yWindow="8243" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -18,14 +18,15 @@
     <sheet name="ZWNL Treinseries" sheetId="1" r:id="rId3"/>
     <sheet name="ZWNL Goederenverbindingen" sheetId="4" r:id="rId4"/>
     <sheet name="ZvNL Treinseries" sheetId="3" r:id="rId5"/>
-    <sheet name="HSL Scenarios" sheetId="7" r:id="rId6"/>
-    <sheet name="HSL Treinseries" sheetId="5" r:id="rId7"/>
-    <sheet name="HSL Standard Scenarios" sheetId="8" r:id="rId8"/>
-    <sheet name="HSL Opmerkingen" sheetId="9" r:id="rId9"/>
+    <sheet name="ZvNL Standard Scenarios" sheetId="11" r:id="rId6"/>
+    <sheet name="HSL Scenarios" sheetId="7" r:id="rId7"/>
+    <sheet name="HSL Treinseries" sheetId="5" r:id="rId8"/>
+    <sheet name="HSL Standard Scenarios" sheetId="8" r:id="rId9"/>
+    <sheet name="HSL Opmerkingen" sheetId="9" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goederenspots!$A$1:$F$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'HSL Treinseries'!$A$1:$G$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ZvNL Treinseries'!$A$1:$F$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ZWNL Goederenverbindingen'!$A$20:$E$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ZWNL Treinseries'!$A$1:$F$30</definedName>
@@ -364,7 +365,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="354">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1507,6 +1508,44 @@
   </si>
   <si>
     <t>Dolime 47628</t>
+  </si>
+  <si>
+    <t>6427 Autumn OC</t>
+  </si>
+  <si>
+    <t>OK
+- Tb 2 ipv 1
+- Bet 3 ipv 4
+- Ehs 3 ipv 4</t>
+  </si>
+  <si>
+    <t>Tbu-Tb:
+- 1100 Tb3 (ipv 2)</t>
+  </si>
+  <si>
+    <t>- 3600 defect Tb1
+- 3900 Btl-Ehv</t>
+  </si>
+  <si>
+    <t>Tb-Btl:
+- 6400 Btl-Ot</t>
+  </si>
+  <si>
+    <t>Btl-Ehv:
+- 800 Bet-Btl
+- 4400 Bet-Btl
+- 1100 Bet-Btl
+- 3500 At-Btl
+- 6400 Ehs-Btl
+- Cargo (1900) Ehv-Btl
+- 3900 Ehv-Btl
+- 800 Ehv-Btl
+- 4400 Ehv-Ehs</t>
+  </si>
+  <si>
+    <t>- Tbu: Fccpps
+- Beto: Klmos
+- Ehv</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1713,6 +1752,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2471,11 +2520,34 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63515A09-7DDE-4638-8E31-255375D1CA8A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="122.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B64A02-8D48-40E3-B121-B38BAF0C0B33}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
@@ -5367,6 +5439,108 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5E853D-4742-4143-BC8A-1A21DC5C0893}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.1328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="35" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="B5" s="35" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B6" s="34"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" s="34"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="34"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B9" s="34"/>
+    </row>
+    <row r="10" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" s="34"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F87682-53E5-48AC-886B-E08EE2D8C03E}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -5474,7 +5648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46531A28-311C-40D4-A423-7F6D69360C5D}">
   <dimension ref="A1:G45"/>
   <sheetViews>
@@ -6409,12 +6583,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB0742C-EC66-4F99-8292-0EC67D49CAE5}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6552,27 +6726,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63515A09-7DDE-4638-8E31-255375D1CA8A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="122.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[6400] Tb-Ehv minor scenario improvements
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F87E268-22AA-4E2C-B807-BE1D0E025DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0942C36A-0796-49E3-86B6-9379780A0DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6885" yWindow="8243" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1635" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -365,7 +365,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="356">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1546,6 +1546,14 @@
     <t>- Tbu: Fccpps
 - Beto: Klmos
 - Ehv</t>
+  </si>
+  <si>
+    <t>- Tbu
+- Tb
+- Ot</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -1686,7 +1694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1752,9 +1760,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5443,7 +5448,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5456,7 +5461,7 @@
       <c r="A1" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>347</v>
       </c>
     </row>
@@ -5464,7 +5469,7 @@
       <c r="A2" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>348</v>
       </c>
     </row>
@@ -5472,37 +5477,37 @@
       <c r="A3" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B6" s="34"/>
+      <c r="B6" s="33"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B7" s="34"/>
+      <c r="B7" s="33"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B8" s="34"/>
+      <c r="B8" s="33"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B9" s="34"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5510,7 +5515,7 @@
       <c r="A11" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5518,21 +5523,30 @@
       <c r="A12" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B12" s="34"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B12" s="33"/>
+    </row>
+    <row r="13" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>195</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>194</v>
       </c>
+      <c r="B14" s="33" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>226</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[6427] Add missing scenario script for weather
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E77486-4542-45FE-8905-DF57E308E732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B54809-591A-47CC-96FC-C77CB658B60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="8115" windowWidth="14400" windowHeight="7485" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -336,40 +336,6 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{EEE704C2-C013-4F27-BFC9-43594913FFA3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-beter afstellen</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Tom</author>
-  </authors>
-  <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D572B1D8-0BA2-43D9-A778-E3F279018DD7}">
       <text>
         <r>
@@ -398,7 +364,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tom</author>
@@ -1779,7 +1745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1850,9 +1816,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5535,11 +5498,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5E853D-4742-4143-BC8A-1A21DC5C0893}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5E853D-4742-4143-BC8A-1A21DC5C0893}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5636,7 +5599,7 @@
       <c r="A15" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5658,7 +5621,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6794,7 +6756,7 @@
       <c r="A10" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="24"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Verwijder cargospots 2022, vervang door sion/somda spots
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D6BB1E-42B5-4553-B872-B0C299892A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A997D30F-E1E0-4EEC-A2C8-3CD91C5E0948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8115" windowWidth="14400" windowHeight="7485" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="8115" windowWidth="14400" windowHeight="7485" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="HSL Treinseries" sheetId="5" r:id="rId8"/>
     <sheet name="HSL Standard Scenarios" sheetId="8" r:id="rId9"/>
     <sheet name="HSL Opmerkingen" sheetId="9" r:id="rId10"/>
+    <sheet name="HvN Standaard Scenarios" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goederenspots!$A$1:$F$51</definedName>
@@ -399,7 +400,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="373">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1641,6 +1642,9 @@
   <si>
     <t>Asd-Awhv Strukton + Klmos
 Asd-Hlm Hagen-Vorhalle staaltrein</t>
+  </si>
+  <si>
+    <t>3255 Spring Fair</t>
   </si>
 </sst>
 </file>
@@ -2634,6 +2638,111 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7076592A-EB7E-42DB-AE68-791BE001EEBD}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.86328125" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B64A02-8D48-40E3-B121-B38BAF0C0B33}">
   <dimension ref="A1:F80"/>
@@ -5534,7 +5643,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6753,7 +6862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB0742C-EC66-4F99-8292-0EC67D49CAE5}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[3235 test] Re-adjust prio's, especially near Ah
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613A6219-A4D6-409C-A492-8E0558B459FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3780219-4851-40D9-ADFB-DB2F5F384006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="14399" windowHeight="7485" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6548" yWindow="4590" windowWidth="14401" windowHeight="7485" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -1685,16 +1685,6 @@
 Let op afwijkende vertrektijd!</t>
   </si>
   <si>
-    <t>Ut:
-- (1)1700
-- 3000 (Utza)
-- 3500
-- 4900/5700
-- 5500
-- 6000/8800
-- 7400</t>
-  </si>
-  <si>
     <t>Ut-Klp:
 - 6900
 - 7300
@@ -1714,23 +1704,33 @@
 - 3000</t>
   </si>
   <si>
-    <t>- 123 Ut-Ah
-- 3600 Ah
-- 3100 Ah</t>
+    <t>- Groene VIRM 9556 3000 Ah v10:26 (Utza?)</t>
+  </si>
+  <si>
+    <t>- Chengdu Shuttle (Wf)
+- Novara shuttle (Mrn)</t>
+  </si>
+  <si>
+    <t>Ut:
+- (1)1700 v07
+- 3000 (Utza) a07
+- 3500 a05
+- 4900/5700 a05
+- 5500 v07
+- 6000/8800 a05
+- 7400 a05</t>
   </si>
   <si>
     <t>Ah:
 - 6600 (perron?)
-- 7600
-- 30700 (tijd?)
-- 31100 (perron?)</t>
-  </si>
-  <si>
-    <t>- Groene VIRM 9556 3000 Ah v10:26 (Utza?)</t>
-  </si>
-  <si>
-    <t>- Chengdu Shuttle (Wf)
-- Novara shuttle (Mrn)</t>
+- 7600 a36 v41
+- 30700 (tijd?) a40
+- 31100 (perron?) v38</t>
+  </si>
+  <si>
+    <t>- 123 Ut-Ah Ah a35
+- 3600 Ah a37
+- 3100 Ah a40</t>
   </si>
 </sst>
 </file>
@@ -2738,14 +2738,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7076592A-EB7E-42DB-AE68-791BE001EEBD}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16.86328125" customWidth="1"/>
-    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+    <col min="2" max="2" width="21.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -2769,31 +2769,31 @@
         <v>192</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="B4" s="34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="B5" s="34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="B6" s="34" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="B7" s="34" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -2809,7 +2809,7 @@
         <v>355</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="57" x14ac:dyDescent="0.45">
@@ -2817,7 +2817,7 @@
         <v>356</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -2830,7 +2830,7 @@
         <v>193</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
[7059] speler en AI
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3780219-4851-40D9-ADFB-DB2F5F384006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630333BB-4EF7-4C42-A531-EBFDE0E583C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6548" yWindow="4590" windowWidth="14401" windowHeight="7485" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6548" yWindow="4590" windowWidth="14401" windowHeight="7485" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="HSL Standard Scenarios" sheetId="8" r:id="rId9"/>
     <sheet name="HSL Opmerkingen" sheetId="9" r:id="rId10"/>
     <sheet name="HvN Standaard Scenarios" sheetId="12" r:id="rId11"/>
+    <sheet name="ATL Standaard Scenarios" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Goederenspots!$A$1:$F$51</definedName>
@@ -434,7 +435,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="387">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1731,6 +1732,33 @@
     <t>- 123 Ut-Ah Ah a35
 - 3600 Ah a37
 - 3100 Ah a40</t>
+  </si>
+  <si>
+    <t>7059 Spring Fair</t>
+  </si>
+  <si>
+    <t>Apd:
+- (geen)</t>
+  </si>
+  <si>
+    <t>Apd-Dv:
+- 17800 Apda
+- 7000 Twl
+- 1600/1700 Dv</t>
+  </si>
+  <si>
+    <t>Dv-Aml:
+- 140 Aspa
+- 7000 Dvc-Hon
+- 1600/1700 Hon
+- 7000 Rsn-Wdn
+- 7900 Wdn-Aml (ri Dv ivm Bvl)
+- 1600/1700 Aml</t>
+  </si>
+  <si>
+    <t>- 1600/1700 Apdo-Aml
+- 17900 Zl-Hgl (na speler)
+- 31000 Vh-Aml (na speler)</t>
   </si>
 </sst>
 </file>
@@ -2738,8 +2766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7076592A-EB7E-42DB-AE68-791BE001EEBD}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2839,6 +2867,130 @@
       </c>
       <c r="B14" s="35" t="s">
         <v>353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31540D39-7427-479F-AD5F-4EC6972CBBE6}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.3984375" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A4" s="5"/>
+      <c r="B4" s="34" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+      <c r="A5" s="5"/>
+      <c r="B5" s="34" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="5"/>
+      <c r="B6" s="35"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="5"/>
+      <c r="B7" s="35"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="5"/>
+      <c r="B8" s="35"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="5"/>
+      <c r="B9" s="35"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
[7059] Goederentreinen en opstel
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089D91D8-9DBF-4EC3-BA96-C8AF3B5DBE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769D2CA4-82AB-4F0C-873A-08D9C3095A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4590" windowWidth="14400" windowHeight="7485" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1761,17 +1761,15 @@
 - 31000 Vh-Aml (na speler)</t>
   </si>
   <si>
-    <t>- Strukton G1206 Dv achter 1600/1700 (ri Amf?)
-- 6414 DBC Aml GDST</t>
-  </si>
-  <si>
-    <t>Apdo https://sion-rail.nl/viewtopic.php?p=198411&amp;hilit=apd#p198411 PCC
-Apdo https://sion-rail.nl/viewtopic.php?p=196114&amp;hilit=rsn#p196114 Hagen-Vorhalle?
-Dv https://sion-rail.nl/viewtopic.php?p=199417&amp;hilit=hon#p199417 Rzepin
-Dvc https://sion-rail.nl/viewtopic.php?p=198203&amp;hilit=apd#p198203 Sweden Xpress
-Dvc-Hon https://sion-rail.nl/viewtopic.php?p=198473&amp;hilit=apd#p198473 Fccpps, Rzepin
-Hon-Rsn https://sion-rail.nl/viewtopic.php?p=196118&amp;hilit=rsn#p196118 PCC, Zonnebloemolietrein
-Aml https://sion-rail.nl/viewtopic.php?p=198472&amp;hilit=rsn#p198472 Rzepin</t>
+    <t>- Apd
+- Dv
+- Aml</t>
+  </si>
+  <si>
+    <t>- Apdo PCC voor 140
+- Dv.34 Rzepin tussen 1600/1700 en 140
+- Dvge.36 Sweden Xpress voor 140
+- Hon-Rsn(.52) Zonnebloemolietrein tussen 1600/1700 en 140</t>
   </si>
 </sst>
 </file>
@@ -1912,7 +1910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1992,12 +1990,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2922,7 +2914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31540D39-7427-479F-AD5F-4EC6972CBBE6}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2984,25 +2976,26 @@
       <c r="A9" s="5"/>
       <c r="B9" s="35"/>
     </row>
-    <row r="10" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B10" s="39" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="B10" s="36"/>
+    </row>
+    <row r="11" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="36" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>206</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
@@ -3017,6 +3010,7 @@
       <c r="A14" s="5" t="s">
         <v>210</v>
       </c>
+      <c r="B14" s="35"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">

</xml_diff>

<commit_message>
[7059 tempdump?] finalize scenario
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769D2CA4-82AB-4F0C-873A-08D9C3095A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E57605-92B9-4522-B6E4-B879DE003B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4590" windowWidth="14400" windowHeight="7485" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="338" yWindow="4928" windowWidth="14400" windowHeight="7485" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -435,7 +435,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="389">
   <si>
     <t>Treinserie</t>
   </si>
@@ -2915,7 +2915,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2928,7 +2928,7 @@
       <c r="A1" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="35" t="s">
         <v>382</v>
       </c>
     </row>
@@ -3016,25 +3016,40 @@
       <c r="A15" s="5" t="s">
         <v>195</v>
       </c>
+      <c r="B15" s="34" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B16" s="34" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B17" s="35" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B18" s="35" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>362</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[7059] Fix player destinationboard
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E57605-92B9-4522-B6E4-B879DE003B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BA5FA3-5D84-4470-9A6C-7598831E0A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="338" yWindow="4928" windowWidth="14400" windowHeight="7485" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goederentreinen" sheetId="2" r:id="rId1"/>
@@ -435,7 +435,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="390">
   <si>
     <t>Treinserie</t>
   </si>
@@ -1770,6 +1770,9 @@
 - Dv.34 Rzepin tussen 1600/1700 en 140
 - Dvge.36 Sweden Xpress voor 140
 - Hon-Rsn(.52) Zonnebloemolietrein tussen 1600/1700 en 140</t>
+  </si>
+  <si>
+    <t>Aml spotten</t>
   </si>
 </sst>
 </file>
@@ -2912,27 +2915,31 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31540D39-7427-479F-AD5F-4EC6972CBBE6}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.3984375" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>190</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>209</v>
       </c>
@@ -2940,7 +2947,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>192</v>
       </c>
@@ -2948,41 +2955,41 @@
         <v>383</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.45">
       <c r="A4" s="5"/>
       <c r="B4" s="34" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="114" x14ac:dyDescent="0.45">
       <c r="A5" s="5"/>
       <c r="B5" s="34" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="B6" s="35"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="5"/>
       <c r="B7" s="35"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="B8" s="35"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
       <c r="B9" s="35"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>355</v>
       </c>
       <c r="B10" s="36"/>
     </row>
-    <row r="11" spans="1:2" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>356</v>
       </c>
@@ -2990,7 +2997,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>206</v>
       </c>
@@ -2998,7 +3005,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>193</v>
       </c>
@@ -3006,13 +3013,13 @@
         <v>386</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>210</v>
       </c>
       <c r="B14" s="35"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>195</v>
       </c>
@@ -3020,7 +3027,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>194</v>
       </c>

</xml_diff>

<commit_message>
ZvNL 2022 Pax consists
</commit_message>
<xml_diff>
--- a/overzicht-2022.xlsx
+++ b/overzicht-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC1C885-3128-4726-BB3F-D1BA21D62868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F5DDF2-4A07-4E1D-A581-14BA72400E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="338" yWindow="2377" windowWidth="21502" windowHeight="12975" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5582,8 +5582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA394F4-D495-45BA-A765-8FE37C144B84}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5783,7 +5783,7 @@
         <v>422</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -5815,7 +5815,7 @@
       </c>
       <c r="D24" s="15">
         <f>$B$21*C24/(B24*24*250)</f>
-        <v>0.31</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="E24" t="s">
         <v>170</v>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="D25" s="15">
         <f t="shared" ref="D25:D33" si="0">$B$21*C25/(B25*24*250)</f>
-        <v>0.34722222222222221</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E25" t="s">
         <v>171</v>
@@ -5853,7 +5853,7 @@
       </c>
       <c r="D26" s="15">
         <f t="shared" si="0"/>
-        <v>0.23749999999999999</v>
+        <v>0.35625000000000001</v>
       </c>
       <c r="E26" t="s">
         <v>172</v>
@@ -5872,7 +5872,7 @@
       </c>
       <c r="D27" s="15">
         <f t="shared" si="0"/>
-        <v>0.11388888888888889</v>
+        <v>0.17083333333333334</v>
       </c>
       <c r="E27" t="s">
         <v>173</v>
@@ -5890,7 +5890,7 @@
       </c>
       <c r="D28" s="15">
         <f t="shared" si="0"/>
-        <v>8.611111111111111E-2</v>
+        <v>0.12916666666666668</v>
       </c>
       <c r="E28" t="s">
         <v>174</v>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="D29" s="15">
         <f t="shared" si="0"/>
-        <v>2.6190476190476191E-2</v>
+        <v>3.9285714285714285E-2</v>
       </c>
       <c r="E29" t="s">
         <v>176</v>
@@ -5927,7 +5927,7 @@
       </c>
       <c r="D30" s="15">
         <f t="shared" si="0"/>
-        <v>0.18333333333333332</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="E30" t="s">
         <v>175</v>
@@ -5945,7 +5945,7 @@
       </c>
       <c r="D31" s="15">
         <f t="shared" si="0"/>
-        <v>9.166666666666666E-2</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="E31" t="s">
         <v>177</v>
@@ -5964,7 +5964,7 @@
       </c>
       <c r="D32" s="15">
         <f t="shared" si="0"/>
-        <v>1.4583333333333334E-2</v>
+        <v>2.1874999999999999E-2</v>
       </c>
       <c r="E32" t="s">
         <v>178</v>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="D33" s="15">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E33" t="s">
         <v>179</v>

</xml_diff>